<commit_message>
Added and styled merged cells
</commit_message>
<xml_diff>
--- a/ExcelFiles/SmallerSampleData.xlsx
+++ b/ExcelFiles/SmallerSampleData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FKANE\source\repos\BenchmarkingExcelPackages\ExcelFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aashraf1\source\repos\BenchmarkingExcelPackages\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2BED0D87-F888-451B-BF30-35066A433EBF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1583E8D5-8EF4-485F-B36E-88F558B10EE9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" activeTab="1" xr2:uid="{CEB28293-C357-4AC2-ACCB-F8B1F9783F0F}"/>
+    <workbookView xWindow="3308" yWindow="3308" windowWidth="16875" windowHeight="10522" activeTab="1" xr2:uid="{CEB28293-C357-4AC2-ACCB-F8B1F9783F0F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -498,15 +498,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{505148EC-0906-4252-8EBE-87FC0CA118CE}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -522,8 +522,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -539,8 +542,11 @@
       <c r="E2" s="3">
         <v>44270</v>
       </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -555,6 +561,9 @@
       </c>
       <c r="E3" s="3">
         <v>44271</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>